<commit_message>
Se soluciono el error, estaba en BAU_FIX (10 y 15)
El problema es que cambiaba el fijo de GSL y DSL, pero NO ESTABA cambiando el fijo de ETH y BDSL, por lo que tomaba el natural
</commit_message>
<xml_diff>
--- a/Exported_files/BAU_Error_Fix15.xlsx
+++ b/Exported_files/BAU_Error_Fix15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\Exported_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37FCC66-9279-48EF-9EE3-991A0D6704EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89C361F-1E30-4087-B832-CC03D9F9FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="28">
   <si>
     <t>Sum of Pv</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Unsaved_12846</t>
+  </si>
+  <si>
+    <t>Unsaved_141929</t>
+  </si>
+  <si>
+    <t>fix_15</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -262,6 +268,8 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -395,10 +403,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U90"/>
+  <dimension ref="A1:U129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87:M90"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G126" sqref="G126:M126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3132,6 +3140,1284 @@
       <c r="M90" s="11">
         <f t="shared" si="13"/>
         <v>6.3168836032160197E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98">
+        <v>2019</v>
+      </c>
+      <c r="F98">
+        <v>2020</v>
+      </c>
+      <c r="G98">
+        <v>2023</v>
+      </c>
+      <c r="H98">
+        <v>2025</v>
+      </c>
+      <c r="I98">
+        <v>2027</v>
+      </c>
+      <c r="J98">
+        <v>2030</v>
+      </c>
+      <c r="K98">
+        <v>2033</v>
+      </c>
+      <c r="L98">
+        <v>2035</v>
+      </c>
+      <c r="M98">
+        <v>2037</v>
+      </c>
+      <c r="N98">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" t="s">
+        <v>27</v>
+      </c>
+      <c r="E99">
+        <v>16.2585882402064</v>
+      </c>
+      <c r="F99">
+        <v>16.011548115260499</v>
+      </c>
+      <c r="G99">
+        <v>16.930945137474701</v>
+      </c>
+      <c r="H99">
+        <v>17.9670453574359</v>
+      </c>
+      <c r="I99">
+        <v>19.125297215971099</v>
+      </c>
+      <c r="J99">
+        <v>20.387477368037398</v>
+      </c>
+      <c r="K99">
+        <v>20.672191753056399</v>
+      </c>
+      <c r="L99">
+        <v>20.792247015017502</v>
+      </c>
+      <c r="M99">
+        <v>21.0260704971524</v>
+      </c>
+      <c r="N99">
+        <v>21.278888943117099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100">
+        <v>16.2585882402064</v>
+      </c>
+      <c r="F100">
+        <v>16.011548115260499</v>
+      </c>
+      <c r="G100">
+        <v>16.930945137474701</v>
+      </c>
+      <c r="H100">
+        <v>17.9670453574359</v>
+      </c>
+      <c r="I100">
+        <v>19.125297215971099</v>
+      </c>
+      <c r="J100">
+        <v>20.387477368037398</v>
+      </c>
+      <c r="K100">
+        <v>20.672191753056399</v>
+      </c>
+      <c r="L100">
+        <v>20.792247015017502</v>
+      </c>
+      <c r="M100">
+        <v>21.0260704971524</v>
+      </c>
+      <c r="N100">
+        <v>21.278888943117099</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" t="s">
+        <v>27</v>
+      </c>
+      <c r="E101">
+        <v>1.2209937579301999E-2</v>
+      </c>
+      <c r="F101">
+        <v>1.14262889191863E-2</v>
+      </c>
+      <c r="G101">
+        <v>1.6926902722401001E-2</v>
+      </c>
+      <c r="H101">
+        <v>2.1137581014534699E-2</v>
+      </c>
+      <c r="I101">
+        <v>2.25557038125253E-2</v>
+      </c>
+      <c r="J101">
+        <v>2.4625104850266099E-2</v>
+      </c>
+      <c r="K101">
+        <v>2.69701469970841E-2</v>
+      </c>
+      <c r="L101">
+        <v>2.8502098352932E-2</v>
+      </c>
+      <c r="M101">
+        <v>3.0279936361084399E-2</v>
+      </c>
+      <c r="N101">
+        <v>3.29101868559631E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" t="s">
+        <v>17</v>
+      </c>
+      <c r="E102">
+        <v>1.2209937579301999E-2</v>
+      </c>
+      <c r="F102">
+        <v>1.14262889191863E-2</v>
+      </c>
+      <c r="G102">
+        <v>1.28481640079312E-2</v>
+      </c>
+      <c r="H102">
+        <v>1.37599485320307E-2</v>
+      </c>
+      <c r="I102">
+        <v>1.46831050984814E-2</v>
+      </c>
+      <c r="J102">
+        <v>1.6030224797365801E-2</v>
+      </c>
+      <c r="K102">
+        <v>1.7556778816175699E-2</v>
+      </c>
+      <c r="L102">
+        <v>1.8554034452738202E-2</v>
+      </c>
+      <c r="M102">
+        <v>1.97113551259811E-2</v>
+      </c>
+      <c r="N102">
+        <v>2.1423571458161799E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103" t="s">
+        <v>27</v>
+      </c>
+      <c r="E103">
+        <v>1.2659383134368299E-2</v>
+      </c>
+      <c r="F103">
+        <v>8.9889111013266004E-3</v>
+      </c>
+      <c r="G103">
+        <v>1.31994925836293E-2</v>
+      </c>
+      <c r="H103">
+        <v>1.6313468094550799E-2</v>
+      </c>
+      <c r="I103">
+        <v>1.6989914140825301E-2</v>
+      </c>
+      <c r="J103">
+        <v>1.79952689290407E-2</v>
+      </c>
+      <c r="K103">
+        <v>1.8646917932001801E-2</v>
+      </c>
+      <c r="L103">
+        <v>1.9057458929770999E-2</v>
+      </c>
+      <c r="M103">
+        <v>1.9468348099935501E-2</v>
+      </c>
+      <c r="N103">
+        <v>2.0039984680446599E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>17</v>
+      </c>
+      <c r="E104">
+        <v>1.2659383134368299E-2</v>
+      </c>
+      <c r="F104">
+        <v>8.9889111013266004E-3</v>
+      </c>
+      <c r="G104">
+        <v>9.9576730270502702E-3</v>
+      </c>
+      <c r="H104">
+        <v>1.06195917690672E-2</v>
+      </c>
+      <c r="I104">
+        <v>1.1059938409254301E-2</v>
+      </c>
+      <c r="J104">
+        <v>1.1714395044228901E-2</v>
+      </c>
+      <c r="K104">
+        <v>1.2138599532695599E-2</v>
+      </c>
+      <c r="L104">
+        <v>1.2405849744330901E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" t="s">
+        <v>27</v>
+      </c>
+      <c r="E105">
+        <v>14.3366332761608</v>
+      </c>
+      <c r="F105">
+        <v>14.7287341880987</v>
+      </c>
+      <c r="G105">
+        <v>20.753469594817901</v>
+      </c>
+      <c r="H105">
+        <v>25.160191914717299</v>
+      </c>
+      <c r="I105">
+        <v>25.624780827354599</v>
+      </c>
+      <c r="J105">
+        <v>26.2822097672389</v>
+      </c>
+      <c r="K105">
+        <v>26.3994965145206</v>
+      </c>
+      <c r="L105">
+        <v>26.453390537439901</v>
+      </c>
+      <c r="M105">
+        <v>26.405545963340099</v>
+      </c>
+      <c r="N105">
+        <v>26.2919819152456</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" t="s">
+        <v>17</v>
+      </c>
+      <c r="E106">
+        <v>14.3366332761608</v>
+      </c>
+      <c r="F106">
+        <v>14.7287341880987</v>
+      </c>
+      <c r="G106">
+        <v>15.7255547191834</v>
+      </c>
+      <c r="H106">
+        <v>16.3785508646647</v>
+      </c>
+      <c r="I106">
+        <v>16.680984691981301</v>
+      </c>
+      <c r="J106">
+        <v>17.108951750749998</v>
+      </c>
+      <c r="K106">
+        <v>17.1853020012813</v>
+      </c>
+      <c r="L106">
+        <v>17.220385437793901</v>
+      </c>
+      <c r="M106">
+        <v>17.1892400159646</v>
+      </c>
+      <c r="N106">
+        <v>17.115313133990899</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" t="s">
+        <v>27</v>
+      </c>
+      <c r="E107">
+        <v>14.3615025968745</v>
+      </c>
+      <c r="F107">
+        <v>14.7491493881192</v>
+      </c>
+      <c r="G107">
+        <v>20.783595990123899</v>
+      </c>
+      <c r="H107">
+        <v>25.1976429638264</v>
+      </c>
+      <c r="I107">
+        <v>25.664326445307999</v>
+      </c>
+      <c r="J107">
+        <v>26.3248301410182</v>
+      </c>
+      <c r="K107">
+        <v>26.4451135794497</v>
+      </c>
+      <c r="L107">
+        <v>26.500950094722601</v>
+      </c>
+      <c r="M107">
+        <v>26.455294247801099</v>
+      </c>
+      <c r="N107">
+        <v>26.344932086781998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" t="s">
+        <v>17</v>
+      </c>
+      <c r="E108">
+        <v>14.3615025968745</v>
+      </c>
+      <c r="F108">
+        <v>14.7491493881192</v>
+      </c>
+      <c r="G108">
+        <v>15.7483605562183</v>
+      </c>
+      <c r="H108">
+        <v>16.402930404965801</v>
+      </c>
+      <c r="I108">
+        <v>16.706727735489</v>
+      </c>
+      <c r="J108">
+        <v>17.136696370591601</v>
+      </c>
+      <c r="K108">
+        <v>17.214997379630098</v>
+      </c>
+      <c r="L108">
+        <v>17.251345321991</v>
+      </c>
+      <c r="M108">
+        <v>17.2089513710905</v>
+      </c>
+      <c r="N108">
+        <v>17.136736705449099</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" t="s">
+        <v>27</v>
+      </c>
+      <c r="E109">
+        <v>22.046268251744099</v>
+      </c>
+      <c r="F109">
+        <v>21.827628563294699</v>
+      </c>
+      <c r="G109">
+        <v>21.786466182217801</v>
+      </c>
+      <c r="H109">
+        <v>21.904867494100898</v>
+      </c>
+      <c r="I109">
+        <v>22.528644666490202</v>
+      </c>
+      <c r="J109">
+        <v>23.2940962613186</v>
+      </c>
+      <c r="K109">
+        <v>24.163484456779798</v>
+      </c>
+      <c r="L109">
+        <v>24.851980359770401</v>
+      </c>
+      <c r="M109">
+        <v>25.284147776300401</v>
+      </c>
+      <c r="N109">
+        <v>25.751422891896599</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110">
+        <v>22.046268251744099</v>
+      </c>
+      <c r="F110">
+        <v>21.827628563294699</v>
+      </c>
+      <c r="G110">
+        <v>21.786466182217801</v>
+      </c>
+      <c r="H110">
+        <v>21.904867494100898</v>
+      </c>
+      <c r="I110">
+        <v>22.528644666490202</v>
+      </c>
+      <c r="J110">
+        <v>23.2940962613186</v>
+      </c>
+      <c r="K110">
+        <v>24.163484456779798</v>
+      </c>
+      <c r="L110">
+        <v>24.851980359770401</v>
+      </c>
+      <c r="M110">
+        <v>25.284147776300401</v>
+      </c>
+      <c r="N110">
+        <v>25.751422891896599</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" t="s">
+        <v>27</v>
+      </c>
+      <c r="E111">
+        <v>0.19969006242069801</v>
+      </c>
+      <c r="F111">
+        <v>0.18687371108081399</v>
+      </c>
+      <c r="G111">
+        <v>0.20604933573894901</v>
+      </c>
+      <c r="H111">
+        <v>0.21766241898546501</v>
+      </c>
+      <c r="I111">
+        <v>0.23226541629233899</v>
+      </c>
+      <c r="J111">
+        <v>0.25357489514973403</v>
+      </c>
+      <c r="K111">
+        <v>0.277722764574731</v>
+      </c>
+      <c r="L111">
+        <v>0.29349790164706802</v>
+      </c>
+      <c r="M111">
+        <v>0.31180503533245402</v>
+      </c>
+      <c r="N111">
+        <v>0.33888981314403699</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112">
+        <v>0.19969006242069801</v>
+      </c>
+      <c r="F112">
+        <v>0.18687371108081399</v>
+      </c>
+      <c r="G112">
+        <v>0.210128074453418</v>
+      </c>
+      <c r="H112">
+        <v>0.22504005146796899</v>
+      </c>
+      <c r="I112">
+        <v>0.24013801500638299</v>
+      </c>
+      <c r="J112">
+        <v>0.26216977520263401</v>
+      </c>
+      <c r="K112">
+        <v>0.28713613275563898</v>
+      </c>
+      <c r="L112">
+        <v>0.303445965547262</v>
+      </c>
+      <c r="M112">
+        <v>0.32237361656755698</v>
+      </c>
+      <c r="N112">
+        <v>0.35037642854183798</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" t="s">
+        <v>27</v>
+      </c>
+      <c r="E113">
+        <v>0.20704061686563099</v>
+      </c>
+      <c r="F113">
+        <v>0.14701108889867301</v>
+      </c>
+      <c r="G113">
+        <v>0.15961309558298301</v>
+      </c>
+      <c r="H113">
+        <v>0.16798653190544899</v>
+      </c>
+      <c r="I113">
+        <v>0.17495217677484101</v>
+      </c>
+      <c r="J113">
+        <v>0.18530473107095899</v>
+      </c>
+      <c r="K113">
+        <v>0.19201503052369501</v>
+      </c>
+      <c r="L113">
+        <v>0.19624254107022801</v>
+      </c>
+      <c r="M113">
+        <v>0.20047363689200001</v>
+      </c>
+      <c r="N113">
+        <v>0.206360015319554</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114">
+        <v>0.20704061686563099</v>
+      </c>
+      <c r="F114">
+        <v>0.14701108889867301</v>
+      </c>
+      <c r="G114">
+        <v>0.16285491513956199</v>
+      </c>
+      <c r="H114">
+        <v>0.173680408230933</v>
+      </c>
+      <c r="I114">
+        <v>0.18088215250641199</v>
+      </c>
+      <c r="J114">
+        <v>0.19158560495577101</v>
+      </c>
+      <c r="K114">
+        <v>0.198523348923002</v>
+      </c>
+      <c r="L114">
+        <v>0.20289415025566901</v>
+      </c>
+      <c r="M114">
+        <v>0.207268658385898</v>
+      </c>
+      <c r="N114">
+        <v>0.21335455465807501</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s">
+        <v>13</v>
+      </c>
+      <c r="D115" t="s">
+        <v>27</v>
+      </c>
+      <c r="E115">
+        <v>234.471566723839</v>
+      </c>
+      <c r="F115">
+        <v>240.884265811901</v>
+      </c>
+      <c r="G115">
+        <v>252.159067701335</v>
+      </c>
+      <c r="H115">
+        <v>259.08490808528302</v>
+      </c>
+      <c r="I115">
+        <v>263.86897237763998</v>
+      </c>
+      <c r="J115">
+        <v>270.63879023276098</v>
+      </c>
+      <c r="K115">
+        <v>271.84654040581597</v>
+      </c>
+      <c r="L115">
+        <v>272.40150946256</v>
+      </c>
+      <c r="M115">
+        <v>271.90883408373003</v>
+      </c>
+      <c r="N115">
+        <v>270.73941808475399</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116">
+        <v>234.471566723839</v>
+      </c>
+      <c r="F116">
+        <v>240.884265811901</v>
+      </c>
+      <c r="G116">
+        <v>257.18698257697002</v>
+      </c>
+      <c r="H116">
+        <v>267.86654913533499</v>
+      </c>
+      <c r="I116">
+        <v>272.81276851301402</v>
+      </c>
+      <c r="J116">
+        <v>279.81204824924998</v>
+      </c>
+      <c r="K116">
+        <v>281.06073491905499</v>
+      </c>
+      <c r="L116">
+        <v>281.63451456220599</v>
+      </c>
+      <c r="M116">
+        <v>281.12514003110499</v>
+      </c>
+      <c r="N116">
+        <v>279.91608686600898</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>3</v>
+      </c>
+      <c r="B117" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" t="s">
+        <v>27</v>
+      </c>
+      <c r="E117">
+        <v>234.878297403125</v>
+      </c>
+      <c r="F117">
+        <v>241.21815061188099</v>
+      </c>
+      <c r="G117">
+        <v>252.524730132657</v>
+      </c>
+      <c r="H117">
+        <v>259.47055703617298</v>
+      </c>
+      <c r="I117">
+        <v>264.27618997070698</v>
+      </c>
+      <c r="J117">
+        <v>271.07766985898201</v>
+      </c>
+      <c r="K117">
+        <v>272.31627820091501</v>
+      </c>
+      <c r="L117">
+        <v>272.89124990527802</v>
+      </c>
+      <c r="M117">
+        <v>272.42111275595403</v>
+      </c>
+      <c r="N117">
+        <v>271.28466791321802</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" t="s">
+        <v>17</v>
+      </c>
+      <c r="E118">
+        <v>234.878297403125</v>
+      </c>
+      <c r="F118">
+        <v>241.21815061188099</v>
+      </c>
+      <c r="G118">
+        <v>257.55996556656299</v>
+      </c>
+      <c r="H118">
+        <v>268.265269595034</v>
+      </c>
+      <c r="I118">
+        <v>273.233788680526</v>
+      </c>
+      <c r="J118">
+        <v>280.26580362940803</v>
+      </c>
+      <c r="K118">
+        <v>281.54639440073402</v>
+      </c>
+      <c r="L118">
+        <v>282.14085467800902</v>
+      </c>
+      <c r="M118">
+        <v>281.65478230605902</v>
+      </c>
+      <c r="N118">
+        <v>280.47981784920898</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" t="s">
+        <v>27</v>
+      </c>
+      <c r="E122" s="17">
+        <f>+E101/E111</f>
+        <v>6.1144442699299952E-2</v>
+      </c>
+      <c r="F122" s="17">
+        <f t="shared" ref="F122:M122" si="14">+F101/F111</f>
+        <v>6.1144442699299598E-2</v>
+      </c>
+      <c r="G122" s="18">
+        <f t="shared" si="14"/>
+        <v>8.2149756327515061E-2</v>
+      </c>
+      <c r="H122" s="18">
+        <f t="shared" si="14"/>
+        <v>9.7111761934182209E-2</v>
+      </c>
+      <c r="I122" s="18">
+        <f t="shared" si="14"/>
+        <v>9.7111761934182E-2</v>
+      </c>
+      <c r="J122" s="18">
+        <f t="shared" si="14"/>
+        <v>9.7111761934181862E-2</v>
+      </c>
+      <c r="K122" s="18">
+        <f t="shared" si="14"/>
+        <v>9.711176193418182E-2</v>
+      </c>
+      <c r="L122" s="18">
+        <f t="shared" si="14"/>
+        <v>9.7111761934181889E-2</v>
+      </c>
+      <c r="M122" s="18">
+        <f t="shared" si="14"/>
+        <v>9.7111761934181737E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" t="s">
+        <v>17</v>
+      </c>
+      <c r="E123" s="17">
+        <f t="shared" ref="E123:M129" si="15">+E102/E112</f>
+        <v>6.1144442699299952E-2</v>
+      </c>
+      <c r="F123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299598E-2</v>
+      </c>
+      <c r="G123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299709E-2</v>
+      </c>
+      <c r="H123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299764E-2</v>
+      </c>
+      <c r="I123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299882E-2</v>
+      </c>
+      <c r="J123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299938E-2</v>
+      </c>
+      <c r="K123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299764E-2</v>
+      </c>
+      <c r="L123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299598E-2</v>
+      </c>
+      <c r="M123" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699300014E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D124" t="s">
+        <v>27</v>
+      </c>
+      <c r="E124" s="17">
+        <f t="shared" si="15"/>
+        <v>6.11444426993E-2</v>
+      </c>
+      <c r="F124" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299931E-2</v>
+      </c>
+      <c r="G124" s="18">
+        <f t="shared" si="15"/>
+        <v>8.2696802135303935E-2</v>
+      </c>
+      <c r="H124" s="18">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181806E-2</v>
+      </c>
+      <c r="I124" s="18">
+        <f t="shared" si="15"/>
+        <v>9.7111761934182084E-2</v>
+      </c>
+      <c r="J124" s="18">
+        <f t="shared" si="15"/>
+        <v>9.7111761934182611E-2</v>
+      </c>
+      <c r="K124" s="18">
+        <f t="shared" si="15"/>
+        <v>9.7111761934182222E-2</v>
+      </c>
+      <c r="L124" s="18">
+        <f t="shared" si="15"/>
+        <v>9.7111761934182417E-2</v>
+      </c>
+      <c r="M124" s="18">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181751E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>12</v>
+      </c>
+      <c r="D125" t="s">
+        <v>17</v>
+      </c>
+      <c r="E125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.11444426993E-2</v>
+      </c>
+      <c r="F125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299931E-2</v>
+      </c>
+      <c r="G125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299743E-2</v>
+      </c>
+      <c r="H125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299334E-2</v>
+      </c>
+      <c r="I125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299716E-2</v>
+      </c>
+      <c r="J125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.114444269930018E-2</v>
+      </c>
+      <c r="K125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299813E-2</v>
+      </c>
+      <c r="L125" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299917E-2</v>
+      </c>
+      <c r="M125" s="17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>13</v>
+      </c>
+      <c r="D126" t="s">
+        <v>27</v>
+      </c>
+      <c r="E126" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299702E-2</v>
+      </c>
+      <c r="F126" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299875E-2</v>
+      </c>
+      <c r="G126" s="17">
+        <f t="shared" si="15"/>
+        <v>8.2303086634976583E-2</v>
+      </c>
+      <c r="H126" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181487E-2</v>
+      </c>
+      <c r="I126" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181917E-2</v>
+      </c>
+      <c r="J126" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181987E-2</v>
+      </c>
+      <c r="K126" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934182042E-2</v>
+      </c>
+      <c r="L126" s="17">
+        <f t="shared" si="15"/>
+        <v>9.711176193418182E-2</v>
+      </c>
+      <c r="M126" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181695E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127" t="s">
+        <v>17</v>
+      </c>
+      <c r="E127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299702E-2</v>
+      </c>
+      <c r="F127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299875E-2</v>
+      </c>
+      <c r="G127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299958E-2</v>
+      </c>
+      <c r="H127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299931E-2</v>
+      </c>
+      <c r="I127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299709E-2</v>
+      </c>
+      <c r="J127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299875E-2</v>
+      </c>
+      <c r="K127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299986E-2</v>
+      </c>
+      <c r="L127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299736E-2</v>
+      </c>
+      <c r="M127" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699300042E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128" t="s">
+        <v>27</v>
+      </c>
+      <c r="E128" s="17">
+        <f t="shared" si="15"/>
+        <v>6.114444269929991E-2</v>
+      </c>
+      <c r="F128" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299695E-2</v>
+      </c>
+      <c r="G128" s="17">
+        <f t="shared" si="15"/>
+        <v>8.2303210379457897E-2</v>
+      </c>
+      <c r="H128" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181917E-2</v>
+      </c>
+      <c r="I128" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934182181E-2</v>
+      </c>
+      <c r="J128" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181834E-2</v>
+      </c>
+      <c r="K128" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181876E-2</v>
+      </c>
+      <c r="L128" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181542E-2</v>
+      </c>
+      <c r="M128" s="17">
+        <f t="shared" si="15"/>
+        <v>9.7111761934181778E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129" t="s">
+        <v>17</v>
+      </c>
+      <c r="E129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.114444269929991E-2</v>
+      </c>
+      <c r="F129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299695E-2</v>
+      </c>
+      <c r="G129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299639E-2</v>
+      </c>
+      <c r="H129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299917E-2</v>
+      </c>
+      <c r="I129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299757E-2</v>
+      </c>
+      <c r="J129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299986E-2</v>
+      </c>
+      <c r="K129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1144442699299639E-2</v>
+      </c>
+      <c r="L129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.114444269929982E-2</v>
+      </c>
+      <c r="M129" s="17">
+        <f t="shared" si="15"/>
+        <v>6.1099446741829017E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>